<commit_message>
Updated Ethanol Folder with corrected Temperatures
</commit_message>
<xml_diff>
--- a/Ethanol/Ethanol_AVE_MASS_FRAC.xlsx
+++ b/Ethanol/Ethanol_AVE_MASS_FRAC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Git_Repos\Pool_Fires\Ethanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{6B8FDB0F-A8A9-4D64-B3FA-81878CAE2B3F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{DF717784-70D6-44B7-87AB-033C1B0EA00D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="11055" xr2:uid="{2C1E920C-970B-4109-9775-1D5AF6DAF90F}"/>
+    <workbookView xWindow="25200" yWindow="-11550" windowWidth="16200" windowHeight="10980" xr2:uid="{2C1E920C-970B-4109-9775-1D5AF6DAF90F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,19 +610,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>6.5792579971812995E-2</v>
+        <v>7.7650977849269817E-2</v>
       </c>
       <c r="C2">
-        <v>2.013374763827775E-3</v>
+        <v>2.295196542455219E-3</v>
       </c>
       <c r="D2">
-        <v>9.6448517728695574E-2</v>
+        <v>0.10744183029275578</v>
       </c>
       <c r="E2">
-        <v>6.3148219054188839E-3</v>
+        <v>7.4888766449407547E-3</v>
       </c>
       <c r="F2">
-        <v>1.8614795438172856E-2</v>
+        <v>2.2146447326846425E-2</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -631,34 +631,34 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.40501964204609781</v>
+        <v>0.46538946313854235</v>
       </c>
       <c r="J2">
-        <v>0.32353941022079152</v>
+        <v>0.2343748911147219</v>
       </c>
       <c r="K2">
-        <v>5.2693689704127224E-3</v>
+        <v>6.178127487171072E-3</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>4.3715232800922883E-2</v>
+        <v>5.2032017840304118E-2</v>
       </c>
       <c r="N2">
-        <v>2.2636909633802143E-2</v>
+        <v>1.6932368035751037E-2</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>8.7712178416543682E-4</v>
+        <v>6.2143403694252177E-4</v>
       </c>
       <c r="Q2">
-        <v>6.8164174191738633E-4</v>
+        <v>4.8065731868859288E-4</v>
       </c>
       <c r="R2">
-        <v>9.0765829939618049E-3</v>
+        <v>6.9677123716103276E-3</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -666,19 +666,19 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>7.8565549653085029E-2</v>
+        <v>8.8263440384111477E-2</v>
       </c>
       <c r="C3">
-        <v>2.56641876340611E-3</v>
+        <v>2.8179217619136339E-3</v>
       </c>
       <c r="D3">
-        <v>0.1051613528302566</v>
+        <v>0.12255206607055497</v>
       </c>
       <c r="E3">
-        <v>7.9584568438273769E-3</v>
+        <v>8.9394414153531696E-3</v>
       </c>
       <c r="F3">
-        <v>2.4089312714349616E-2</v>
+        <v>2.6900451809774916E-2</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -687,34 +687,34 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.51504923913437728</v>
+        <v>0.5598731259137949</v>
       </c>
       <c r="J3">
-        <v>0.1729404147583711</v>
+        <v>9.6301838351008376E-2</v>
       </c>
       <c r="K3">
-        <v>4.8557930702327569E-3</v>
+        <v>9.2042520986496453E-3</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>5.3291261319955194E-2</v>
+        <v>5.9865686843953922E-2</v>
       </c>
       <c r="N3">
-        <v>2.339271862568203E-2</v>
+        <v>1.6670157757145233E-2</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>1.0890155678767797E-3</v>
+        <v>7.1433700159036532E-4</v>
       </c>
       <c r="Q3">
-        <v>6.5174915479839E-4</v>
+        <v>4.2827958251172407E-4</v>
       </c>
       <c r="R3">
-        <v>1.0388717563781761E-2</v>
+        <v>7.4690010096376278E-3</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -722,19 +722,19 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8.9018543910947337E-2</v>
+        <v>9.5287438272993782E-2</v>
       </c>
       <c r="C4">
-        <v>2.4209898821857989E-3</v>
+        <v>2.5434322278413018E-3</v>
       </c>
       <c r="D4">
-        <v>0.11412140129938592</v>
+        <v>0.1154708949988751</v>
       </c>
       <c r="E4">
-        <v>9.1463051069259893E-3</v>
+        <v>9.7726810599756964E-3</v>
       </c>
       <c r="F4">
-        <v>2.9724378633389531E-2</v>
+        <v>3.1601634040896359E-2</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -743,34 +743,34 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0.58952662607887207</v>
+        <v>0.6095917336643093</v>
       </c>
       <c r="J4">
-        <v>6.6875729028400346E-2</v>
+        <v>4.363583023651358E-2</v>
       </c>
       <c r="K4">
-        <v>8.5737100279474864E-3</v>
+        <v>9.0725149215348019E-3</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>5.604358971798664E-2</v>
+        <v>5.9615535336234364E-2</v>
       </c>
       <c r="N4">
-        <v>2.2917891204865211E-2</v>
+        <v>1.553961581292968E-2</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>1.0509279102201628E-3</v>
+        <v>6.7114124664696196E-4</v>
       </c>
       <c r="Q4">
-        <v>6.0205714159048058E-4</v>
+        <v>3.7620800673437602E-4</v>
       </c>
       <c r="R4">
-        <v>9.97785005728293E-3</v>
+        <v>6.8213401745146097E-3</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -778,19 +778,19 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>8.7675060136578317E-2</v>
+        <v>9.1756517114560787E-2</v>
       </c>
       <c r="C5">
-        <v>1.7971064240566116E-3</v>
+        <v>1.7365967378778189E-3</v>
       </c>
       <c r="D5">
-        <v>0.11319319523265306</v>
+        <v>0.10684336666692139</v>
       </c>
       <c r="E5">
-        <v>1.018478918689374E-2</v>
+        <v>1.0713486432351168E-2</v>
       </c>
       <c r="F5">
-        <v>4.8671307665157905E-2</v>
+        <v>5.1182742407965803E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -799,34 +799,34 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.65106986901965147</v>
+        <v>0.66058954418115745</v>
       </c>
       <c r="J5">
-        <v>1.6460414377057732E-2</v>
+        <v>1.1108883206032259E-2</v>
       </c>
       <c r="K5">
-        <v>6.0347462708542328E-3</v>
+        <v>6.2023408613692379E-3</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>4.3391383317096112E-2</v>
+        <v>4.5212093447173404E-2</v>
       </c>
       <c r="N5">
-        <v>1.3715322221282564E-2</v>
+        <v>9.4433982378554285E-3</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>7.7144688038758896E-4</v>
+        <v>5.3702381212209925E-4</v>
       </c>
       <c r="Q5">
-        <v>3.7388654840026051E-4</v>
+        <v>2.3844864651348271E-4</v>
       </c>
       <c r="R5">
-        <v>6.6614727199304433E-3</v>
+        <v>4.4355582480997083E-3</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -834,19 +834,19 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>7.7335729069117315E-2</v>
+        <v>7.9713082848292233E-2</v>
       </c>
       <c r="C6">
-        <v>1.4046133051762223E-3</v>
+        <v>1.4330728065518248E-3</v>
       </c>
       <c r="D6">
-        <v>8.5617680444270261E-2</v>
+        <v>8.4488738168766647E-2</v>
       </c>
       <c r="E6">
-        <v>1.0794401882608743E-2</v>
+        <v>1.1199782240325801E-2</v>
       </c>
       <c r="F6">
-        <v>6.9648838918731887E-2</v>
+        <v>7.1896651146980878E-2</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -855,34 +855,34 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.69255906353199637</v>
+        <v>0.69539153922957353</v>
       </c>
       <c r="J6">
-        <v>9.1121498242565536E-3</v>
+        <v>5.7761367918317376E-3</v>
       </c>
       <c r="K6">
-        <v>4.4788708782449553E-3</v>
+        <v>4.6019546562011794E-3</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>3.4957369716318985E-2</v>
+        <v>3.6160433844838344E-2</v>
       </c>
       <c r="N6">
-        <v>8.7991344186918972E-3</v>
+        <v>5.8589985020059765E-3</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>3.9361056870677549E-4</v>
+        <v>2.4419956388441769E-4</v>
       </c>
       <c r="Q6">
-        <v>2.9228978679603478E-4</v>
+        <v>1.7734380374179957E-4</v>
       </c>
       <c r="R6">
-        <v>4.6062476550840286E-3</v>
+        <v>3.0580663970055195E-3</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -890,19 +890,19 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>5.9802997450709668E-2</v>
+        <v>6.7253411155698606E-2</v>
       </c>
       <c r="C7">
-        <v>4.3158893194731462E-4</v>
+        <v>5.7863736106888563E-4</v>
       </c>
       <c r="D7">
-        <v>4.2305712162277548E-2</v>
+        <v>5.809569063464963E-2</v>
       </c>
       <c r="E7">
-        <v>1.1601114572604824E-2</v>
+        <v>1.170222505602906E-2</v>
       </c>
       <c r="F7">
-        <v>0.121860531521763</v>
+        <v>0.11096195447465579</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -911,22 +911,22 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0.74242420237115636</v>
+        <v>0.72739077718590006</v>
       </c>
       <c r="J7">
-        <v>1.3591194598732289E-3</v>
+        <v>1.1239602370112481E-3</v>
       </c>
       <c r="K7">
-        <v>1.514529096573645E-3</v>
+        <v>1.9153446624747194E-3</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1.3892346610798285E-2</v>
+        <v>1.7193818265629542E-2</v>
       </c>
       <c r="N7">
-        <v>3.2402580904230677E-3</v>
+        <v>2.5360880986783027E-3</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -935,10 +935,10 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1.2978689769938112E-4</v>
+        <v>8.5107857982037993E-5</v>
       </c>
       <c r="R7">
-        <v>1.437812834173831E-3</v>
+        <v>1.1629850102219822E-3</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -946,19 +946,19 @@
         <v>30</v>
       </c>
       <c r="B8">
-        <v>5.3873418336153098E-2</v>
+        <v>5.3929007797550818E-2</v>
       </c>
       <c r="C8">
-        <v>1.7153711008079556E-4</v>
+        <v>1.7033429176696452E-4</v>
       </c>
       <c r="D8">
-        <v>2.8144451636188669E-2</v>
+        <v>4.1518131044865604E-2</v>
       </c>
       <c r="E8">
-        <v>1.1743089432000205E-2</v>
+        <v>1.18935167730075E-2</v>
       </c>
       <c r="F8">
-        <v>0.14177798143363077</v>
+        <v>0.14280719567999819</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -967,22 +967,22 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0.75605059497400606</v>
+        <v>0.74197615175252507</v>
       </c>
       <c r="J8">
-        <v>2.1351322269226402E-4</v>
+        <v>1.3150727049635277E-4</v>
       </c>
       <c r="K8">
-        <v>5.0660183595045444E-4</v>
+        <v>5.1464200237591191E-4</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>5.8619460400354245E-3</v>
+        <v>5.9870608844036291E-3</v>
       </c>
       <c r="N8">
-        <v>1.2464352963347518E-3</v>
+        <v>7.9529589593393827E-4</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -991,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>1.4902274340089092E-5</v>
+        <v>1.4086821208677452E-5</v>
       </c>
       <c r="R8">
-        <v>3.9552840858735229E-4</v>
+        <v>2.6306978586730444E-4</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1002,19 +1002,19 @@
         <v>45</v>
       </c>
       <c r="B9">
-        <v>3.2780077372710534E-2</v>
+        <v>3.3242976412738948E-2</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1.9491489352083363E-2</v>
+        <v>2.1168619157900498E-2</v>
       </c>
       <c r="E9">
-        <v>1.1780388888469509E-2</v>
+        <v>1.1955650000754879E-2</v>
       </c>
       <c r="F9">
-        <v>0.1762847415116568</v>
+        <v>0.17964657220773519</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1023,19 +1023,19 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0.75885459336151051</v>
+        <v>0.75351287490926955</v>
       </c>
       <c r="J9">
-        <v>1.4504026146111945E-5</v>
+        <v>9.0038145856967015E-6</v>
       </c>
       <c r="K9">
-        <v>2.15425225956803E-5</v>
+        <v>2.1709072341432119E-5</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>6.1624083124680847E-4</v>
+        <v>3.4008612768205479E-4</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>1.564221335805333E-4</v>
+        <v>1.0250829699170914E-4</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1058,19 +1058,19 @@
         <v>60</v>
       </c>
       <c r="B10">
-        <v>1.9683246372609625E-2</v>
+        <v>2.0073044886322281E-2</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1.5897515754171119E-2</v>
+        <v>1.2944034505505192E-2</v>
       </c>
       <c r="E10">
-        <v>1.1767550138534045E-2</v>
+        <v>1.2141731555582434E-2</v>
       </c>
       <c r="F10">
-        <v>0.19521459097087546</v>
+        <v>0.20270824766078444</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1079,19 +1079,19 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.75743709676380966</v>
+        <v>0.75210310613450371</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1.0209353094297727E-5</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1.9625904207698935E-5</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1202,19 +1202,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5.3279650586735804E-3</v>
+        <v>6.0854384124294121E-3</v>
       </c>
       <c r="C2">
-        <v>2.5721821899577331E-4</v>
+        <v>2.03061726349037E-4</v>
       </c>
       <c r="D2">
-        <v>2.1125747187649098E-2</v>
+        <v>2.2023274547215602E-2</v>
       </c>
       <c r="E2">
-        <v>8.077642260364222E-4</v>
+        <v>1.0255830932353865E-3</v>
       </c>
       <c r="F2">
-        <v>7.419862562891605E-3</v>
+        <v>8.3302052743043069E-3</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1223,34 +1223,34 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>4.8737127291045054E-2</v>
+        <v>5.2654665694891058E-2</v>
       </c>
       <c r="J2">
-        <v>0.15913123121651016</v>
+        <v>0.11228507448389466</v>
       </c>
       <c r="K2">
-        <v>4.896256057201581E-4</v>
+        <v>5.6339607663276337E-4</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>3.744984732390363E-3</v>
+        <v>4.7873504517861772E-3</v>
       </c>
       <c r="N2">
-        <v>4.1692576612598377E-3</v>
+        <v>3.2283518853831496E-3</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>5.1836831740199472E-4</v>
+        <v>2.8891284009774262E-4</v>
       </c>
       <c r="Q2">
-        <v>6.0743064495573661E-5</v>
+        <v>4.6898734430133737E-5</v>
       </c>
       <c r="R2">
-        <v>1.3135870749869005E-3</v>
+        <v>1.0714781846085442E-3</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1258,19 +1258,19 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>6.5680726194916042E-3</v>
+        <v>8.8524209316939162E-3</v>
       </c>
       <c r="C3">
-        <v>5.1593078808527743E-4</v>
+        <v>5.5416065245914091E-4</v>
       </c>
       <c r="D3">
-        <v>2.2209522263142361E-2</v>
+        <v>3.3987479616525512E-2</v>
       </c>
       <c r="E3">
-        <v>7.0977606609511123E-4</v>
+        <v>9.5609334241487009E-4</v>
       </c>
       <c r="F3">
-        <v>1.9309830246733876E-2</v>
+        <v>2.1465242817737092E-2</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1279,34 +1279,34 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>4.6460694256997739E-2</v>
+        <v>4.8811032714784708E-2</v>
       </c>
       <c r="J3">
-        <v>4.8450197909765659E-2</v>
+        <v>3.9008751422410136E-2</v>
       </c>
       <c r="K3">
-        <v>3.7268255242377661E-3</v>
+        <v>2.6170880608307068E-3</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>1.1319818973560408E-2</v>
+        <v>1.2668045467365984E-2</v>
       </c>
       <c r="N3">
-        <v>6.2655675414268431E-3</v>
+        <v>4.4865863742205182E-3</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>5.0348799086123979E-4</v>
+        <v>1.5683845986274485E-4</v>
       </c>
       <c r="Q3">
-        <v>1.9710557211560529E-4</v>
+        <v>1.3154169593135483E-4</v>
       </c>
       <c r="R3">
-        <v>2.7791334309847883E-3</v>
+        <v>2.0393836793288068E-3</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1314,19 +1314,19 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>3.0502643653422703E-3</v>
+        <v>4.4079630298698973E-3</v>
       </c>
       <c r="C4">
-        <v>1.1583515874371481E-4</v>
+        <v>1.5391509782393262E-4</v>
       </c>
       <c r="D4">
-        <v>2.7521997616423346E-2</v>
+        <v>3.6014999045295953E-2</v>
       </c>
       <c r="E4">
-        <v>3.6297234536837147E-4</v>
+        <v>7.8327552523534735E-4</v>
       </c>
       <c r="F4">
-        <v>1.0959991677378014E-3</v>
+        <v>1.6302779230136398E-3</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1335,34 +1335,34 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1.8544140695884666E-2</v>
+        <v>2.7084795877457882E-2</v>
       </c>
       <c r="J4">
-        <v>1.5294295773448974E-2</v>
+        <v>8.497893378592164E-3</v>
       </c>
       <c r="K4">
-        <v>7.7995772942866413E-4</v>
+        <v>9.2272181881775952E-4</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1.9569529827014103E-3</v>
+        <v>2.676127108047177E-3</v>
       </c>
       <c r="N4">
-        <v>1.8746417681174503E-3</v>
+        <v>1.5175312650972436E-3</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>5.3188108860449917E-4</v>
+        <v>1.8995409501206833E-4</v>
       </c>
       <c r="Q4">
-        <v>4.0540685883036505E-5</v>
+        <v>2.9627595365873751E-5</v>
       </c>
       <c r="R4">
-        <v>5.5941810019434013E-4</v>
+        <v>4.6730123102439719E-4</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1370,19 +1370,19 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>2.9597771273653668E-3</v>
+        <v>4.5668406785444324E-3</v>
       </c>
       <c r="C5">
-        <v>3.3587529646605967E-4</v>
+        <v>4.436437291757716E-4</v>
       </c>
       <c r="D5">
-        <v>2.4063927051639632E-2</v>
+        <v>2.0798768914459604E-2</v>
       </c>
       <c r="E5">
-        <v>6.2432522735179506E-4</v>
+        <v>1.0523905286749257E-3</v>
       </c>
       <c r="F5">
-        <v>1.5203081736380497E-2</v>
+        <v>1.6443486514894828E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1391,34 +1391,34 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>3.5078757922475015E-2</v>
+        <v>4.8538962792641076E-2</v>
       </c>
       <c r="J5">
-        <v>4.2574406783020763E-3</v>
+        <v>2.5520288486608131E-3</v>
       </c>
       <c r="K5">
-        <v>1.0065482461825478E-3</v>
+        <v>1.088596957443091E-3</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>7.6816941363622498E-3</v>
+        <v>7.7556596722893993E-3</v>
       </c>
       <c r="N5">
-        <v>1.2285766938723332E-3</v>
+        <v>6.8678432351284375E-4</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>3.6447159985258416E-4</v>
+        <v>1.4845374855898826E-4</v>
       </c>
       <c r="Q5">
-        <v>3.9204725959481073E-5</v>
+        <v>4.0665997843380784E-5</v>
       </c>
       <c r="R5">
-        <v>1.3894589360545378E-3</v>
+        <v>8.4807760215003885E-4</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1426,19 +1426,19 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>1.2053513198548535E-2</v>
+        <v>1.2567529737204958E-2</v>
       </c>
       <c r="C6">
-        <v>1.1140162989092782E-3</v>
+        <v>1.1380323161611884E-3</v>
       </c>
       <c r="D6">
-        <v>1.6350920617768539E-2</v>
+        <v>1.8735108498394423E-2</v>
       </c>
       <c r="E6">
-        <v>7.1756095300216547E-4</v>
+        <v>1.0471437536660785E-3</v>
       </c>
       <c r="F6">
-        <v>4.6972029034275935E-2</v>
+        <v>4.8488105066337661E-2</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1447,34 +1447,34 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>4.5662370284373408E-2</v>
+        <v>4.7632013639611233E-2</v>
       </c>
       <c r="J6">
-        <v>1.158893077970089E-2</v>
+        <v>7.3085470611360401E-3</v>
       </c>
       <c r="K6">
-        <v>3.4287830614916082E-3</v>
+        <v>3.5258331228958874E-3</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2.3450312853217886E-2</v>
+        <v>2.4281521895849967E-2</v>
       </c>
       <c r="N6">
-        <v>4.8320477754287853E-3</v>
+        <v>3.2795987926104906E-3</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>2.9437741816124371E-4</v>
+        <v>1.4932676024025438E-4</v>
       </c>
       <c r="Q6">
-        <v>5.5270373935960475E-5</v>
+        <v>3.3800210097645087E-5</v>
       </c>
       <c r="R6">
-        <v>3.7408814918203598E-3</v>
+        <v>2.4862407313451353E-3</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1482,19 +1482,19 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>1.2918170768511674E-2</v>
+        <v>1.6313339045567433E-3</v>
       </c>
       <c r="C7">
-        <v>2.6374773960533552E-4</v>
+        <v>2.765393325942855E-5</v>
       </c>
       <c r="D7">
-        <v>3.9770700456095445E-2</v>
+        <v>1.102171382077682E-2</v>
       </c>
       <c r="E7">
-        <v>4.5345990792454297E-4</v>
+        <v>8.2979112546681161E-4</v>
       </c>
       <c r="F7">
-        <v>2.4593720368580704E-2</v>
+        <v>2.3895743913142009E-3</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1503,22 +1503,22 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2.3052411584109488E-2</v>
+        <v>1.5551085334641232E-2</v>
       </c>
       <c r="J7">
-        <v>9.2316373074333678E-4</v>
+        <v>1.002582755334319E-4</v>
       </c>
       <c r="K7">
-        <v>7.7927528532857496E-4</v>
+        <v>1.0104146687145279E-4</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>6.1434921745720517E-3</v>
+        <v>4.0929596616772824E-4</v>
       </c>
       <c r="N7">
-        <v>1.3359575864120127E-3</v>
+        <v>3.9322038916370988E-5</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -1527,10 +1527,10 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>2.7298403389224186E-5</v>
+        <v>3.7503707853534392E-6</v>
       </c>
       <c r="R7">
-        <v>7.0309754758112744E-4</v>
+        <v>6.3430885460600777E-5</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1538,19 +1538,19 @@
         <v>30</v>
       </c>
       <c r="B8">
-        <v>1.5834074975019645E-3</v>
+        <v>2.2191814466303371E-3</v>
       </c>
       <c r="C8">
-        <v>4.4213150172844332E-5</v>
+        <v>4.2330919110245834E-5</v>
       </c>
       <c r="D8">
-        <v>6.6035539325961252E-3</v>
+        <v>1.2527150507768722E-2</v>
       </c>
       <c r="E8">
-        <v>4.1560326997799575E-4</v>
+        <v>9.5366824485095566E-4</v>
       </c>
       <c r="F8">
-        <v>8.005608566397638E-3</v>
+        <v>1.0797938089490413E-2</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1559,22 +1559,22 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1.9229891856065245E-2</v>
+        <v>3.3998121747070432E-2</v>
       </c>
       <c r="J8">
-        <v>1.6442155263441955E-4</v>
+        <v>9.8677994649125857E-5</v>
       </c>
       <c r="K8">
-        <v>1.6515037752624261E-4</v>
+        <v>1.6096998566692458E-4</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>1.5559987712367581E-3</v>
+        <v>1.5135767352856199E-3</v>
       </c>
       <c r="N8">
-        <v>4.1837977617685697E-4</v>
+        <v>2.5997814127629693E-4</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -1583,10 +1583,10 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>2.9818318495340176E-5</v>
+        <v>2.8190353332233043E-5</v>
       </c>
       <c r="R8">
-        <v>1.3543867502493437E-4</v>
+        <v>9.3734850346650212E-5</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1594,19 +1594,19 @@
         <v>45</v>
       </c>
       <c r="B9">
-        <v>2.8495039071843994E-3</v>
+        <v>3.3655534399250511E-3</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>3.7178059333668437E-3</v>
+        <v>5.4989565239554053E-3</v>
       </c>
       <c r="E9">
-        <v>7.4439557496279842E-4</v>
+        <v>8.845308428185282E-4</v>
       </c>
       <c r="F9">
-        <v>9.3949780674024465E-3</v>
+        <v>8.9765025241268434E-3</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1615,19 +1615,19 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>3.8773205622090204E-2</v>
+        <v>2.4884511144939093E-2</v>
       </c>
       <c r="J9">
-        <v>1.0778868188672789E-5</v>
+        <v>6.5138348049137553E-6</v>
       </c>
       <c r="K9">
-        <v>5.0396520750000577E-6</v>
+        <v>4.8315652616327985E-6</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>4.1551895052804621E-5</v>
+        <v>6.8026281944652588E-4</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>3.1304765620806418E-4</v>
+        <v>2.0516726322287302E-4</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1650,19 +1650,19 @@
         <v>60</v>
       </c>
       <c r="B10">
-        <v>1.8188872300457179E-3</v>
+        <v>1.8715828853326263E-3</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>3.01793907618243E-3</v>
+        <v>2.8302195079080296E-3</v>
       </c>
       <c r="E10">
-        <v>5.1329555784766832E-4</v>
+        <v>9.8300279107332422E-4</v>
       </c>
       <c r="F10">
-        <v>4.0262305150694988E-3</v>
+        <v>9.5255871993857547E-3</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1671,19 +1671,19 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1.9488515560554014E-2</v>
+        <v>2.35997853645207E-2</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>2.0433009624408887E-5</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>3.9257565520056565E-5</v>
       </c>
       <c r="N10">
         <v>0</v>

</xml_diff>